<commit_message>
Updated code for SIT env
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23655" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23661" uniqueCount="958">
   <si>
     <t>transactionName</t>
   </si>
@@ -2887,6 +2887,18 @@
   </si>
   <si>
     <t>TS28EcommTransaction_3d53e4</t>
+  </si>
+  <si>
+    <t>REF1689584053702</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_d07803</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_700b35</t>
+  </si>
+  <si>
+    <t>07-18-2023</t>
   </si>
 </sst>
 </file>
@@ -3800,10 +3812,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>901</v>
@@ -3842,7 +3854,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>941</v>
+        <v>957</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
@@ -3867,10 +3879,10 @@
     </row>
     <row r="3" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>901</v>
@@ -3909,7 +3921,7 @@
         <v>10</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>941</v>
+        <v>957</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated bulk upload code
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23661" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23566" uniqueCount="916">
   <si>
     <t>transactionName</t>
   </si>
@@ -2718,187 +2718,61 @@
     <t>TS28</t>
   </si>
   <si>
-    <t>PREFNO1</t>
-  </si>
-  <si>
     <t>Creditor1</t>
   </si>
   <si>
-    <t>PREFNO2</t>
-  </si>
-  <si>
-    <t>Creditor2</t>
-  </si>
-  <si>
     <t>Payment</t>
   </si>
   <si>
-    <t>06-22-2023</t>
-  </si>
-  <si>
-    <t>REF1687340710058</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_bc103b</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_a1446f</t>
-  </si>
-  <si>
-    <t>REF1687341368065</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_02df2a</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_024dd3</t>
-  </si>
-  <si>
-    <t>REF1687341762293</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_5d7eb9</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_b84b06</t>
-  </si>
-  <si>
-    <t>REF1687343182309</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_ba8c5b</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_fba1c8</t>
-  </si>
-  <si>
-    <t>REF1687348179960</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_663117</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_e5fb89</t>
-  </si>
-  <si>
-    <t>REF1687354829345</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_e280a2</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_7d7f2d</t>
-  </si>
-  <si>
-    <t>REF1687412155836</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_890959</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_028d1e</t>
-  </si>
-  <si>
-    <t>06-23-2023</t>
-  </si>
-  <si>
-    <t>REF1687412484650</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_ea72a6</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_a4ea6d</t>
-  </si>
-  <si>
-    <t>REF1687414030621</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_d6e3ef</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_bf0dae</t>
-  </si>
-  <si>
-    <t>REF1688476285728</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_a36edb</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_2855c4</t>
-  </si>
-  <si>
-    <t>07-05-2023</t>
-  </si>
-  <si>
-    <t>REF1688476672456</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_0ae53c</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_5f62b0</t>
-  </si>
-  <si>
-    <t>REF1688539133907</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_85674c</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_09e7a3</t>
-  </si>
-  <si>
-    <t>07-06-2023</t>
-  </si>
-  <si>
-    <t>REF1688539675349</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_8e8121</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_1b142d</t>
-  </si>
-  <si>
-    <t>REF1688540731300</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_cc0175</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_a498b0</t>
-  </si>
-  <si>
-    <t>REF1688558367926</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_7f87fd</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_59b48d</t>
-  </si>
-  <si>
-    <t>REF1688558709786</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_85d9e0</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_3d53e4</t>
-  </si>
-  <si>
-    <t>REF1689584053702</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_d07803</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_700b35</t>
-  </si>
-  <si>
-    <t>07-18-2023</t>
+    <t>07-26-2023</t>
+  </si>
+  <si>
+    <t>REF1690286636910</t>
+  </si>
+  <si>
+    <t>PREFNO12894</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_5257rea4</t>
+  </si>
+  <si>
+    <t>REF1690347121608</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_1146e6</t>
+  </si>
+  <si>
+    <t>07-27-2023</t>
+  </si>
+  <si>
+    <t>REF1690347561083</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_1532d4</t>
+  </si>
+  <si>
+    <t>REF1690348251578</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_8a861d</t>
+  </si>
+  <si>
+    <t>REF1690352470308</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_bff938</t>
+  </si>
+  <si>
+    <t>REF1690353527216</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_e2d9bb</t>
+  </si>
+  <si>
+    <t>REF1690355357871</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_c0c882</t>
   </si>
 </sst>
 </file>
@@ -3184,8 +3058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GO1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3812,13 +3686,13 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>955</v>
+        <v>915</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>954</v>
+        <v>914</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>895</v>
@@ -3845,16 +3719,16 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>897</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>898</v>
       </c>
       <c r="P2" s="4">
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>957</v>
+        <v>905</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
@@ -3878,65 +3752,29 @@
       <c r="GE2" s="4"/>
     </row>
     <row r="3" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>956</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>954</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>901</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>896</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>895</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="7" t="s">
-        <v>895</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>197</v>
-      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>900</v>
-      </c>
-      <c r="P3" s="4">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>957</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>201</v>
-      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="6" t="s">
-        <v>202</v>
-      </c>
+      <c r="Z3" s="6"/>
       <c r="AA3" s="3"/>
       <c r="AI3" s="3"/>
       <c r="EQ3" s="3"/>

</xml_diff>

<commit_message>
Added TS69 && Updated TS10_Holiday code
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23661" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23667" uniqueCount="962">
   <si>
     <t>transactionName</t>
   </si>
@@ -2899,6 +2899,18 @@
   </si>
   <si>
     <t>07-18-2023</t>
+  </si>
+  <si>
+    <t>REF1690804669640</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_4e4755</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_0758d9</t>
+  </si>
+  <si>
+    <t>08-01-2023</t>
   </si>
 </sst>
 </file>
@@ -3812,10 +3824,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>901</v>
@@ -3854,7 +3866,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
@@ -3879,10 +3891,10 @@
     </row>
     <row r="3" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>901</v>
@@ -3921,7 +3933,7 @@
         <v>10</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated Account Entitlement && Bulk Upload Testscript
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23670" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23694" uniqueCount="982">
   <si>
     <t>transactionName</t>
   </si>
@@ -2920,6 +2920,57 @@
   </si>
   <si>
     <t>08-04-2023</t>
+  </si>
+  <si>
+    <t>REF1691566959313</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_77aca3</t>
+  </si>
+  <si>
+    <t>08-10-2023</t>
+  </si>
+  <si>
+    <t>REF1691570322822</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_98ca6d</t>
+  </si>
+  <si>
+    <t>REF1691574973531</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_a2e40b</t>
+  </si>
+  <si>
+    <t>REF1691575702557</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_2a6a3d</t>
+  </si>
+  <si>
+    <t>REF1691576626379</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_76f6c5</t>
+  </si>
+  <si>
+    <t>REF1691577197954</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_87f62d</t>
+  </si>
+  <si>
+    <t>REF1691581725478</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_4b7449</t>
+  </si>
+  <si>
+    <t>REF1691582418487</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_e1f311</t>
   </si>
 </sst>
 </file>
@@ -3833,10 +3884,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>963</v>
+        <v>981</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>962</v>
+        <v>980</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>901</v>
@@ -3875,7 +3926,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated TS25 && Updated TS73_Assertion
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23694" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23712" uniqueCount="995">
   <si>
     <t>transactionName</t>
   </si>
@@ -2971,6 +2971,45 @@
   </si>
   <si>
     <t>TS28EcommTransaction_e1f311</t>
+  </si>
+  <si>
+    <t>REF1691647052238</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_21e438</t>
+  </si>
+  <si>
+    <t>08-11-2023</t>
+  </si>
+  <si>
+    <t>REF1691648107434</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_efb546</t>
+  </si>
+  <si>
+    <t>REF1691655029052</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_08d307</t>
+  </si>
+  <si>
+    <t>REF1691655719854</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_94f972</t>
+  </si>
+  <si>
+    <t>REF1691656049562</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_8e419d</t>
+  </si>
+  <si>
+    <t>REF1691659179784</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_1e780d</t>
   </si>
 </sst>
 </file>
@@ -3884,10 +3923,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>981</v>
+        <v>994</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>980</v>
+        <v>993</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>901</v>
@@ -3926,7 +3965,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>967</v>
+        <v>984</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated global properties file for QA execution
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23733" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23754" uniqueCount="1028">
   <si>
     <t>transactionName</t>
   </si>
@@ -3061,6 +3061,54 @@
   </si>
   <si>
     <t>08-17-2023</t>
+  </si>
+  <si>
+    <t>REF1692770363993</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_f9a7ee</t>
+  </si>
+  <si>
+    <t>08-24-2023</t>
+  </si>
+  <si>
+    <t>REF1692773441896</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_b3502b</t>
+  </si>
+  <si>
+    <t>REF1692780944361</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_235ef0</t>
+  </si>
+  <si>
+    <t>REF1692783476881</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_722d1f</t>
+  </si>
+  <si>
+    <t>REF1692786249734</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_d2d9fa</t>
+  </si>
+  <si>
+    <t>REF1692786652987</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_1e3e30</t>
+  </si>
+  <si>
+    <t>REF1692940774996</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_261cb6</t>
+  </si>
+  <si>
+    <t>08-26-2023</t>
   </si>
 </sst>
 </file>
@@ -3974,10 +4022,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>1010</v>
+        <v>1026</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1009</v>
+        <v>1025</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>901</v>
@@ -4016,7 +4064,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>1011</v>
+        <v>1027</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated TS10 && Added TS28_Assertion
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23566" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23569" uniqueCount="919">
   <si>
     <t>transactionName</t>
   </si>
@@ -2773,6 +2773,15 @@
   </si>
   <si>
     <t>TS28EcommTransaction_712942</t>
+  </si>
+  <si>
+    <t>REF1693821732375</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_6f5fd2</t>
+  </si>
+  <si>
+    <t>09-05-2023</t>
   </si>
 </sst>
 </file>
@@ -3686,10 +3695,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3728,7 +3737,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Added TS84 && TS87
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23569" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23572" uniqueCount="922">
   <si>
     <t>transactionName</t>
   </si>
@@ -2782,6 +2782,15 @@
   </si>
   <si>
     <t>09-05-2023</t>
+  </si>
+  <si>
+    <t>REF1694409180495</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_0cf866</t>
+  </si>
+  <si>
+    <t>09-12-2023</t>
   </si>
 </sst>
 </file>
@@ -3695,10 +3704,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3737,7 +3746,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Added Rolback transaction Api
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23572" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23581" uniqueCount="929">
   <si>
     <t>transactionName</t>
   </si>
@@ -2791,6 +2791,27 @@
   </si>
   <si>
     <t>09-12-2023</t>
+  </si>
+  <si>
+    <t>REF1694765872728</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_a46ee2</t>
+  </si>
+  <si>
+    <t>09-16-2023</t>
+  </si>
+  <si>
+    <t>REF1694767502685</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_84374b</t>
+  </si>
+  <si>
+    <t>REF1694768520264</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_f23d17</t>
   </si>
 </sst>
 </file>
@@ -3704,10 +3725,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3746,7 +3767,7 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Added TS97 && Updated TS28
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23581" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23552" uniqueCount="907">
   <si>
     <t>transactionName</t>
   </si>
@@ -2727,91 +2727,25 @@
     <t>Payment</t>
   </si>
   <si>
-    <t>09-01-2023</t>
-  </si>
-  <si>
-    <t>REF1693492863823</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_1bb5fe</t>
-  </si>
-  <si>
-    <t>REF1693493743771</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_26c662</t>
-  </si>
-  <si>
-    <t>REF1693540244126</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_5678d8</t>
-  </si>
-  <si>
-    <t>09-02-2023</t>
-  </si>
-  <si>
-    <t>REF1693540939369</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_44d311</t>
-  </si>
-  <si>
-    <t>REF1693542295182</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_b191a9</t>
-  </si>
-  <si>
-    <t>REF1693548907702</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_9448e9</t>
-  </si>
-  <si>
-    <t>REF1693550421866</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_712942</t>
-  </si>
-  <si>
-    <t>REF1693821732375</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_6f5fd2</t>
-  </si>
-  <si>
-    <t>09-05-2023</t>
-  </si>
-  <si>
-    <t>REF1694409180495</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_0cf866</t>
-  </si>
-  <si>
-    <t>09-12-2023</t>
-  </si>
-  <si>
-    <t>REF1694765872728</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_a46ee2</t>
-  </si>
-  <si>
-    <t>09-16-2023</t>
-  </si>
-  <si>
-    <t>REF1694767502685</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_84374b</t>
-  </si>
-  <si>
-    <t>REF1694768520264</t>
-  </si>
-  <si>
-    <t>TS28EcommTransaction_f23d17</t>
+    <t>REF1695363013629</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_a7db21</t>
+  </si>
+  <si>
+    <t>09-23-2023</t>
+  </si>
+  <si>
+    <t>REF1695364618746</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_55c82c</t>
+  </si>
+  <si>
+    <t>09-22-2023</t>
+  </si>
+  <si>
+    <t>12:17PM</t>
   </si>
 </sst>
 </file>
@@ -3097,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GO1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3117,9 +3051,9 @@
     <col min="14" max="14" customWidth="true" width="18.25" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="21.5" collapsed="true"/>
     <col min="16" max="16" customWidth="true" width="8.4140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="10.58203125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="8.4140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.08203125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="13.9140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.83203125" collapsed="true"/>
     <col min="20" max="20" customWidth="true" width="13.4140625" collapsed="true"/>
     <col min="21" max="24" customWidth="true" width="8.4140625" collapsed="true"/>
     <col min="25" max="25" customWidth="true" width="18.83203125" collapsed="true"/>
@@ -3725,10 +3659,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>928</v>
+        <v>904</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>927</v>
+        <v>903</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3767,13 +3701,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>924</v>
+        <v>905</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>200</v>
+        <v>906</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Added TS107 && Updated TS100,TS104
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23568" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23576" uniqueCount="927">
   <si>
     <t>transactionName</t>
   </si>
@@ -2785,6 +2785,27 @@
   </si>
   <si>
     <t>12:02PM</t>
+  </si>
+  <si>
+    <t>REF1697454209137</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_787bc1</t>
+  </si>
+  <si>
+    <t>10-16-2023</t>
+  </si>
+  <si>
+    <t>04:43PM</t>
+  </si>
+  <si>
+    <t>REF1697455025203</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_b11a13</t>
+  </si>
+  <si>
+    <t>04:57PM</t>
   </si>
 </sst>
 </file>
@@ -3698,10 +3719,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>918</v>
+        <v>925</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3740,13 +3761,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>909</v>
+        <v>922</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>919</v>
+        <v>926</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Added TS107 && Updated 97,100,114
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23576" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23584" uniqueCount="933">
   <si>
     <t>transactionName</t>
   </si>
@@ -2806,6 +2806,24 @@
   </si>
   <si>
     <t>04:57PM</t>
+  </si>
+  <si>
+    <t>REF1697694208344</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_c65db7</t>
+  </si>
+  <si>
+    <t>10-19-2023</t>
+  </si>
+  <si>
+    <t>11:23AM</t>
+  </si>
+  <si>
+    <t>REF1697694817218</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_d21402</t>
   </si>
 </sst>
 </file>
@@ -3719,10 +3737,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>925</v>
+        <v>932</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>924</v>
+        <v>931</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3761,13 +3779,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>926</v>
+        <v>910</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Added TS123 && TS124
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23584" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23588" uniqueCount="937">
   <si>
     <t>transactionName</t>
   </si>
@@ -2824,6 +2824,18 @@
   </si>
   <si>
     <t>TS28EcommTransaction_d21402</t>
+  </si>
+  <si>
+    <t>REF1698991484985</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_650387</t>
+  </si>
+  <si>
+    <t>11-03-2023</t>
+  </si>
+  <si>
+    <t>11:43AM</t>
   </si>
 </sst>
 </file>
@@ -3737,10 +3749,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3779,13 +3791,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>929</v>
+        <v>935</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>910</v>
+        <v>936</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Updated testcases for documentdb
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23600" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23608" uniqueCount="954">
   <si>
     <t>transactionName</t>
   </si>
@@ -2866,6 +2866,27 @@
   </si>
   <si>
     <t>03:16PM</t>
+  </si>
+  <si>
+    <t>REF1702550310299</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_eb070b</t>
+  </si>
+  <si>
+    <t>12-14-2023</t>
+  </si>
+  <si>
+    <t>04:18PM</t>
+  </si>
+  <si>
+    <t>REF1702550701370</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_dfcfb3</t>
+  </si>
+  <si>
+    <t>04:24PM</t>
   </si>
 </sst>
 </file>
@@ -3779,10 +3800,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3821,13 +3842,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>939</v>
+        <v>949</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Updated code for documentdb
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23608" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23648" uniqueCount="986">
   <si>
     <t>transactionName</t>
   </si>
@@ -2887,6 +2887,102 @@
   </si>
   <si>
     <t>04:24PM</t>
+  </si>
+  <si>
+    <t>REF1703150762420</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_a80ba8</t>
+  </si>
+  <si>
+    <t>12-21-2023</t>
+  </si>
+  <si>
+    <t>REF1703231286011</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_1897af</t>
+  </si>
+  <si>
+    <t>12-22-2023</t>
+  </si>
+  <si>
+    <t>01:27PM</t>
+  </si>
+  <si>
+    <t>REF1703231883705</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_b47e14</t>
+  </si>
+  <si>
+    <t>01:37PM</t>
+  </si>
+  <si>
+    <t>REF1703567691363</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_ac7499</t>
+  </si>
+  <si>
+    <t>12-26-2023</t>
+  </si>
+  <si>
+    <t>10:55AM</t>
+  </si>
+  <si>
+    <t>REF1703570028851</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_90ec9d</t>
+  </si>
+  <si>
+    <t>11:33AM</t>
+  </si>
+  <si>
+    <t>REF1703576727547</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_8a104f</t>
+  </si>
+  <si>
+    <t>01:25PM</t>
+  </si>
+  <si>
+    <t>REF1703581803737</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_43c8eb</t>
+  </si>
+  <si>
+    <t>02:51PM</t>
+  </si>
+  <si>
+    <t>REF1703585930923</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_486a00</t>
+  </si>
+  <si>
+    <t>03:58PM</t>
+  </si>
+  <si>
+    <t>REF1703588067536</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_0218cf</t>
+  </si>
+  <si>
+    <t>04:33PM</t>
+  </si>
+  <si>
+    <t>REF1703590199091</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_ef091c</t>
+  </si>
+  <si>
+    <t>05:09PM</t>
   </si>
 </sst>
 </file>
@@ -3800,10 +3896,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>952</v>
+        <v>984</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>951</v>
+        <v>983</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>899</v>
@@ -3842,13 +3938,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>949</v>
+        <v>966</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>953</v>
+        <v>985</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
Added ProdIssue Testcases && Updated code for removing wait
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\upp-test-automation\src\main\resources\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23548" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23552" uniqueCount="907">
   <si>
     <t>transactionName</t>
   </si>
@@ -2734,12 +2734,25 @@
   </si>
   <si>
     <t>TS28EcommTransaction_a6334112hf</t>
+  </si>
+  <si>
+    <t>REF1706179709171</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_5a8dcb</t>
+  </si>
+  <si>
+    <t>01-25-2024</t>
+  </si>
+  <si>
+    <t>04:27PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3024,31 +3037,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.25" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.75" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="8.4140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="20.83203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.08203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.25" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.5" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.4140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.08203125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.9140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.83203125" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.4140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="24" width="8.4140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.83203125" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.58203125" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="19.25" customWidth="1" collapsed="1"/>
-    <col min="28" max="32" width="8.4140625" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="19.08203125" customWidth="1" collapsed="1"/>
-    <col min="34" max="197" width="8.4140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.25" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.75" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="8.4140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.75" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.08203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.25" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="8.4140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.08203125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="13.9140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.4140625" collapsed="true"/>
+    <col min="21" max="24" customWidth="true" width="8.4140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="16.58203125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="19.25" collapsed="true"/>
+    <col min="28" max="32" customWidth="true" width="8.4140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="19.08203125" collapsed="true"/>
+    <col min="34" max="197" customWidth="true" width="8.4140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3646,10 +3659,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>898</v>
@@ -3688,13 +3701,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>200</v>
@@ -4753,7 +4766,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="250" width="8.4140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="250" customWidth="true" width="8.4140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added tag && Updated failed testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/BulkEcomm.xlsx
+++ b/src/main/resources/BulkEcomm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23552" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23560" uniqueCount="915">
   <si>
     <t>transactionName</t>
   </si>
@@ -2746,6 +2746,30 @@
   </si>
   <si>
     <t>04:27PM</t>
+  </si>
+  <si>
+    <t>REF1709918774992</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_0f62ef</t>
+  </si>
+  <si>
+    <t>03-08-2024</t>
+  </si>
+  <si>
+    <t>11:05PM</t>
+  </si>
+  <si>
+    <t>REF1710156303568</t>
+  </si>
+  <si>
+    <t>TS28EcommTransaction_a1d8e5</t>
+  </si>
+  <si>
+    <t>03-11-2024</t>
+  </si>
+  <si>
+    <t>05:06PM</t>
   </si>
 </sst>
 </file>
@@ -3659,10 +3683,10 @@
     </row>
     <row r="2" spans="1:197" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>898</v>
@@ -3701,13 +3725,13 @@
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>199</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>200</v>

</xml_diff>